<commit_message>
gc and app update for the test user
</commit_message>
<xml_diff>
--- a/gc.xlsx
+++ b/gc.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H512"/>
+  <dimension ref="A1:H513"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -13668,33 +13668,59 @@
     </row>
     <row r="512">
       <c r="A512" t="str">
-        <v>admin</v>
+        <v>test</v>
       </c>
       <c r="B512" t="str">
-        <v>admin</v>
+        <v>test</v>
       </c>
       <c r="C512" t="str">
-        <v>admin</v>
+        <v>test</v>
       </c>
       <c r="D512" t="str">
         <v>Fri Apr 09 2021 23:55:50 GMT+0530 (India Standard Time)</v>
       </c>
       <c r="E512" t="str">
+        <v>All Good</v>
+      </c>
+      <c r="F512" t="str">
+        <v>test</v>
+      </c>
+      <c r="G512" t="str">
+        <v>30</v>
+      </c>
+      <c r="H512" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="str">
         <v>admin</v>
       </c>
-      <c r="F512" t="str">
+      <c r="B513" t="str">
         <v>admin</v>
       </c>
-      <c r="G512" t="str">
-        <v>0</v>
-      </c>
-      <c r="H512" t="str">
+      <c r="C513" t="str">
+        <v>admin</v>
+      </c>
+      <c r="D513" t="str">
+        <v>Fri Apr 09 2021 23:55:50 GMT+0530 (India Standard Time)</v>
+      </c>
+      <c r="E513" t="str">
+        <v>admin</v>
+      </c>
+      <c r="F513" t="str">
+        <v>admin</v>
+      </c>
+      <c r="G513" t="str">
+        <v>0</v>
+      </c>
+      <c r="H513" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H512"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H513"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>